<commit_message>
Updated Blue Sparrow Excel File
</commit_message>
<xml_diff>
--- a/Excel Project Files/Blue Sparrow Data.xlsx
+++ b/Excel Project Files/Blue Sparrow Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony Ayala\Downloads\Excel School Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B3E1FB-615C-4541-9F66-6181F4556239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AED894-CE72-40B3-9CB3-35202ACEF2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$4</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$5:$E$52</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$5:$E$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -259,6 +257,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Drive Through Wait Time (Sec)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -297,6 +325,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Average Drive Through Wait Time (Sec) Monthly</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -321,6 +352,157 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.064701616245338E-2"/>
+                  <c:y val="7.0964811971117717E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-DB0C-4720-8720-90FCA8D4FAFB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1683243541925679E-2"/>
+                  <c:y val="5.8516679191034732E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-DB0C-4720-8720-90FCA8D4FAFB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.193535018648985E-2"/>
+                  <c:y val="9.5861077531283659E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-DB0C-4720-8720-90FCA8D4FAFB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$G$20:$G$31</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>December</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Janurary</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>July</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$H$20:$H$31</c:f>
@@ -369,7 +551,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-115A-4216-8318-805644D0B10B}"/>
+              <c16:uniqueId val="{00000000-DB0C-4720-8720-90FCA8D4FAFB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -388,8 +570,9 @@
         <c:axId val="650343887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -405,75 +588,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
+        <c:tickLblPos val="low"/>
         <c:crossAx val="624116351"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="624116351"/>
@@ -496,36 +618,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -617,7 +709,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -655,7 +747,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{7A97ED60-D894-4652-BF53-79CB9B649A4F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Avg Drive-Through Wait Time (sec)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1834,8 +1926,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7013575" y="254000"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="7007225" y="247650"/>
+              <a:ext cx="4572000" cy="2695575"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1868,26 +1960,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
+      <xdr:colOff>336550</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>517525</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F12E349C-4D8D-1638-F247-33AB05F1BB8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1E417DB-A099-41D4-A2E4-1D68E13AD80E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2169,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>